<commit_message>
Added data driven framework and did some bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/events.xlsx
+++ b/src/test/resources/testdata/events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="164">
   <si>
     <t>Date</t>
   </si>
@@ -962,10 +962,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>20</v>
@@ -976,10 +976,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>20</v>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>20</v>
@@ -1116,10 +1116,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>20</v>
@@ -1186,10 +1186,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>63</v>
@@ -1200,10 +1200,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>63</v>
@@ -1567,7 +1567,7 @@
         <v>122</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>124</v>
@@ -1581,7 +1581,7 @@
         <v>122</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s" s="0">
         <v>124</v>

</xml_diff>